<commit_message>
+91-ph added in download template
</commit_message>
<xml_diff>
--- a/public/assets/download-format/erp_user.xlsx
+++ b/public/assets/download-format/erp_user.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t xml:space="preserve">user_first_name</t>
   </si>
@@ -118,6 +118,9 @@
     <t xml:space="preserve">singh</t>
   </si>
   <si>
+    <t xml:space="preserve">+91-9651970290</t>
+  </si>
+  <si>
     <t xml:space="preserve">kuvikash123@gmail.com</t>
   </si>
   <si>
@@ -137,6 +140,12 @@
   </si>
   <si>
     <t xml:space="preserve">Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+91-9776687022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+91-9561970290</t>
   </si>
   <si>
     <t xml:space="preserve">Hii</t>
@@ -146,10 +155,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="yyyy/dd/mm;@"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="167" formatCode="YYYY/DD/MM;@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -224,24 +234,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,22 +340,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC1048518"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:AC2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.43"/>
@@ -344,106 +366,106 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="37.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="22.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -457,47 +479,47 @@
       <c r="C2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="5" t="n">
         <v>41187</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>9651970290</v>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>30</v>
       </c>
       <c r="O2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>9776687022</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="S2" s="0" t="s">
         <v>30</v>
@@ -506,13 +528,13 @@
         <v>31</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>9561970290</v>
+        <v>33</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>30</v>
@@ -521,52 +543,48 @@
         <v>31</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>9561970290</v>
+        <v>33</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="4" t="n">
         <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="4"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
+      <c r="D3" s="6"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="4"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
+      <c r="D4" s="6"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="kuvikash123@gmail.com"/>

</xml_diff>